<commit_message>
update interface day 1
</commit_message>
<xml_diff>
--- a/FacebookSDK/Document/Gui-AppPhotoFB (Autosaved).xlsx
+++ b/FacebookSDK/Document/Gui-AppPhotoFB (Autosaved).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5880,7 +5880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update again file Excel
</commit_message>
<xml_diff>
--- a/FacebookSDK/Document/Gui-AppPhotoFB (Autosaved).xlsx
+++ b/FacebookSDK/Document/Gui-AppPhotoFB (Autosaved).xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GUI APP" sheetId="1" r:id="rId1"/>
+    <sheet name="Task Manager" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
@@ -18,9 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Nhiệm vụ</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Duy</t>
+  </si>
+  <si>
+    <t>Quyền</t>
+  </si>
+  <si>
+    <t>Monday, 26/6/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design 2 screen Login and Account Infomation </t>
+  </si>
+  <si>
+    <t>(Task)Account information from FB</t>
+  </si>
+  <si>
+    <t>(Task)Tabbar</t>
+  </si>
+  <si>
+    <t>(Task)Login FB</t>
+  </si>
+  <si>
+    <t>(Task)Datasource for TableView from FB</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,21 +86,104 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="40"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="25"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -89,8 +208,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5192,15 +5336,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>(action) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>load account information</a:t>
+            <a:t>(action) load account information</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5276,15 +5412,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>(action) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>load friend</a:t>
+            <a:t>(action) load friend</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0">
@@ -5383,21 +5511,8 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>(action) </a:t>
+            <a:t>(action) back to album</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>back to album</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5471,15 +5586,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>(action) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>select a</a:t>
+            <a:t>(action) select a</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0">
@@ -5565,23 +5672,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>(action) go to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>album</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> tab</a:t>
+            <a:t>(action) go to album tab</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5878,27 +5969,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="8.83203125" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" customWidth="1"/>
+    <col min="29" max="29" width="49.85546875" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="29:29" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="AC1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="5" customWidth="1"/>
+    <col min="3" max="23" width="52.7109375" style="5" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" s="6" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A20"/>
+    <mergeCell ref="B1:B10"/>
+    <mergeCell ref="B11:B20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>